<commit_message>
Tabel van analyse perfect strategie toegevoegd
</commit_message>
<xml_diff>
--- a/Blackjack/EenVariabele.xlsx
+++ b/Blackjack/EenVariabele.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@data\schoolhogent\2tin\semmester2\Onderzoek\Onderzoekstechnieken\Blackjack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kavoos\Documents\HoGent\Chamilo\Onderzoekstechnieken\project\Blackjack\Onderzoekstechnieken\Blackjack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12204" windowHeight="5952"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Waarnemingen</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>standaardafwijking</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Perfect</t>
   </si>
 </sst>
 </file>
@@ -89,11 +95,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -109,9 +118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +158,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -221,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -371,138 +380,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1039.5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <f>MEDIAN(A2:A11)</f>
+      <c r="C3">
+        <f>MEDIAN(A3:A12)</f>
         <v>1039.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="E3">
+        <v>1021.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>MEDIAN(E3:E12)</f>
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1045</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <f>MODE(A2:A11)</f>
+      <c r="C4">
+        <f>MODE(A3:A12)</f>
         <v>1042</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="E4">
+        <v>1016</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>MODE(E3:E12)</f>
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>1032.5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <f>ABS(MAX(A2:A11)-MIN(A2:A11))</f>
+      <c r="C5">
+        <f>ABS(MAX(A3:A12)-MIN(A3:A12))</f>
         <v>16.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E5">
+        <v>1014</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f>ABS(MAX(E3:E12)-MIN(E3:E12))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1040</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <f>QUARTILE(A2:A11,1)</f>
+      <c r="C6">
+        <f>QUARTILE(A3:A12,1)</f>
         <v>1035.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="E6">
+        <v>1027.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f>QUARTILE(E3:E12,1)</f>
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1042</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <f>QUARTILE(A2:A11,2)</f>
+      <c r="C7">
+        <f>QUARTILE(A3:A12,2)</f>
         <v>1039.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="E7">
+        <v>1022.5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <f>QUARTILE(E3:E12,2)</f>
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>1034.5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <f>QUARTILE(A2:A11,3)</f>
+      <c r="C8">
+        <f>QUARTILE(A3:A12,3)</f>
         <v>1042</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="E8">
+        <v>1017</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <f>QUARTILE(E3:E12,3)</f>
+        <v>1022.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>1035</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <f>VARP(A2:A11)</f>
+      <c r="C9">
+        <f>VARP(A3:A12)</f>
         <v>23.352499999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="E9">
+        <v>1023</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f>VARP(E3:E12)</f>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>1042</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <f>SQRT(C8)</f>
+      <c r="C10">
+        <f>SQRT(C9)</f>
         <v>4.8324424466308962</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="E10">
+        <v>1016</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <f>SQRT(G9)</f>
+        <v>4.2895221179054435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>1037</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="E11">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>1049</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="E12">
+        <v>1013.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C12">
-        <f>AVERAGE(A2:A11)</f>
+      <c r="C13">
+        <f>AVERAGE(A3:A12)</f>
         <v>1039.6500000000001</v>
       </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>AVERAGE(E3:E12)</f>
+        <v>1019</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>